<commit_message>
Requerimientos y tiempos estimados
</commit_message>
<xml_diff>
--- a/Documentacion/Requerimientos_y_Especificaciones.xlsx
+++ b/Documentacion/Requerimientos_y_Especificaciones.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="177">
   <si>
     <t>Nro.</t>
   </si>
@@ -170,9 +170,6 @@
     <t>RD30</t>
   </si>
   <si>
-    <t>Seleccionar</t>
-  </si>
-  <si>
     <t>Web Escritorio</t>
   </si>
   <si>
@@ -444,24 +441,6 @@
   </si>
   <si>
     <t>RD33</t>
-  </si>
-  <si>
-    <t>RD34</t>
-  </si>
-  <si>
-    <t>RD35</t>
-  </si>
-  <si>
-    <t>RD36</t>
-  </si>
-  <si>
-    <t>RD37</t>
-  </si>
-  <si>
-    <t>RD38</t>
-  </si>
-  <si>
-    <t>RD39</t>
   </si>
   <si>
     <t>Modulo REST de cliente final</t>
@@ -1075,7 +1054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1115,7 +1094,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
@@ -1123,61 +1102,61 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="2:5" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="2:5" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="2:5" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="7"/>
     </row>
@@ -1283,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B44" sqref="B39:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1370,28 +1349,28 @@
         <v>19</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -1403,28 +1382,28 @@
         <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="I5" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -1436,28 +1415,28 @@
         <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -1469,28 +1448,28 @@
         <v>20</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -1502,28 +1481,28 @@
         <v>21</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="H8" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -1535,28 +1514,28 @@
         <v>22</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E9" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="H9" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -1568,28 +1547,28 @@
         <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="H10" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -1601,28 +1580,28 @@
         <v>24</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E11" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="G11" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -1634,28 +1613,28 @@
         <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E12" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="H12" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -1667,28 +1646,28 @@
         <v>26</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E13" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="H13" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -1700,28 +1679,28 @@
         <v>27</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>109</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
@@ -1733,28 +1712,28 @@
         <v>28</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E15" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="G15" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
@@ -1766,28 +1745,28 @@
         <v>29</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E16" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="H16" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
@@ -1799,28 +1778,28 @@
         <v>30</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E17" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>113</v>
-      </c>
       <c r="G17" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
@@ -1832,28 +1811,28 @@
         <v>31</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
@@ -1865,28 +1844,28 @@
         <v>32</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="H19" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
@@ -1898,28 +1877,28 @@
         <v>33</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>123</v>
-      </c>
       <c r="G20" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
@@ -1931,28 +1910,28 @@
         <v>34</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E21" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>125</v>
-      </c>
       <c r="G21" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
@@ -1964,28 +1943,28 @@
         <v>35</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E22" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>127</v>
-      </c>
       <c r="G22" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
@@ -1997,28 +1976,28 @@
         <v>36</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="G23" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -2030,28 +2009,28 @@
         <v>37</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
@@ -2063,28 +2042,28 @@
         <v>38</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
@@ -2096,28 +2075,28 @@
         <v>39</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
@@ -2129,28 +2108,28 @@
         <v>40</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -2162,28 +2141,28 @@
         <v>41</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -2195,28 +2174,28 @@
         <v>42</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
@@ -2228,28 +2207,28 @@
         <v>43</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
@@ -2261,28 +2240,28 @@
         <v>44</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
@@ -2294,28 +2273,28 @@
         <v>45</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
@@ -2327,28 +2306,28 @@
         <v>46</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
@@ -2360,28 +2339,28 @@
         <v>47</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -2393,28 +2372,28 @@
         <v>48</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
@@ -2423,31 +2402,31 @@
     </row>
     <row r="36" spans="2:14" ht="36" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
@@ -2456,31 +2435,31 @@
     </row>
     <row r="37" spans="2:14" ht="24" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -2489,47 +2468,41 @@
     </row>
     <row r="38" spans="2:14" ht="24" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C38" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>178</v>
-      </c>
       <c r="F38" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
     </row>
-    <row r="39" spans="2:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>49</v>
-      </c>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -2541,16 +2514,10 @@
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
     </row>
-    <row r="40" spans="2:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>49</v>
-      </c>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -2562,16 +2529,10 @@
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
     </row>
-    <row r="41" spans="2:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>49</v>
-      </c>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -2583,16 +2544,10 @@
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
     </row>
-    <row r="42" spans="2:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>49</v>
-      </c>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -2604,16 +2559,10 @@
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
     </row>
-    <row r="43" spans="2:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>49</v>
-      </c>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B43" s="4"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -2625,16 +2574,10 @@
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
     </row>
-    <row r="44" spans="2:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>49</v>
-      </c>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>

</xml_diff>